<commit_message>
Adds timepix commmad 0x79 to reboot. Corrects command name for cdte3 read_all_hk
</commit_message>
<xml_diff>
--- a/commands/cdte3/cdte3_command_deck.xlsx
+++ b/commands/cdte3/cdte3_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi-4matter/foxsi4-commands/commands/cdte3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254373FC-E6F5-8C41-AA4A-79AF2BE416D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43645722-95F3-CC47-8BE4-6E6134FF5B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17900" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="117">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -382,6 +382,9 @@
   </si>
   <si>
     <t>0x7d</t>
+  </si>
+  <si>
+    <t>read_can3_all_hk</t>
   </si>
 </sst>
 </file>
@@ -859,7 +862,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R31" sqref="R31"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -2185,7 +2188,7 @@
     </row>
     <row r="16" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>35</v>

</xml_diff>